<commit_message>
Update the template Excel
</commit_message>
<xml_diff>
--- a/Template/BPC/BPC_Login.xlsx
+++ b/Template/BPC/BPC_Login.xlsx
@@ -16,28 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Click</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>username</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>by.id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>by.name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>by.xpath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sendkeys</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -50,30 +34,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>input username</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Yes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>No</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>html\table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetValue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>by.id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>$UserName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -82,7 +46,90 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>submit</t>
+    <t>CompareWith</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FieldName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Step</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FieldParameter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IdentifyType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IdentifyAttribute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input user name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Click login button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ById</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ByXpath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ls_usernam</t>
+  </si>
+  <si>
+    <t>ls_password</t>
+  </si>
+  <si>
+    <t>.//*[@id='lsform']/div/div/table/tbody/tr[2]/td[3]/button</t>
+  </si>
+  <si>
+    <t>GetAttribute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Submit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.//*[@id='um']/p[1]/strong/a</t>
+  </si>
+  <si>
+    <t>#DisplayedName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DisplayedName</t>
+  </si>
+  <si>
+    <t>$DisplayedName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -90,79 +137,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CompareWith</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SearchID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GenerateID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>searchID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#BPC_Create:id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>msg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#RecordiId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#mgsContent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$CompareWith</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$BPC_Login:msgContent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VerifyCheckBoc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>checkbox</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FieldName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FieldParameter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IdentifyType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IdentifyAttribute</t>
+    <t>Get the specified attribute value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Verify the displayed name in the page is same as the login name.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -531,15 +510,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="10.125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.75" style="3" customWidth="1"/>
     <col min="3" max="4" width="9" style="3"/>
     <col min="5" max="5" width="13" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.625" style="3" customWidth="1"/>
@@ -550,170 +530,142 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.5">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="2">
-        <v>123</v>
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="28.5">
       <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="42.75">
       <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="28.5">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="2">
-        <v>122</v>
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="36.75" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+    <row r="6" spans="1:8" ht="57">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="36.75" customHeight="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="28.5">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="28.5">
-      <c r="C9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>31</v>
+      <c r="H6" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finally update before the first phase.
</commit_message>
<xml_diff>
--- a/Template/BPC/BPC_Login.xlsx
+++ b/Template/BPC/BPC_Login.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="12765" windowHeight="5715"/>
@@ -22,10 +22,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sendkeys</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>NeedOrNot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -98,19 +94,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ls_usernam</t>
-  </si>
-  <si>
     <t>ls_password</t>
   </si>
   <si>
     <t>.//*[@id='lsform']/div/div/table/tbody/tr[2]/td[3]/button</t>
   </si>
   <si>
-    <t>GetAttribute</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>UserName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -142,14 +131,26 @@
   </si>
   <si>
     <t>Verify the displayed name in the page is same as the login name.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ls_username</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SendKeys</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetText</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,15 +219,20 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -300,6 +306,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -334,6 +341,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -509,14 +517,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.75" style="3" customWidth="1"/>
@@ -528,144 +534,144 @@
     <col min="9" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="28.5">
-      <c r="A2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="28.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="42.75">
+    <row r="4" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="28.5">
+    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="57">
+    <row r="6" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -675,12 +681,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -688,12 +694,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>